<commit_message>
Atualização automática de SANTO_AUGUSTO.xlsx
</commit_message>
<xml_diff>
--- a/SANTO_AUGUSTO.xlsx
+++ b/SANTO_AUGUSTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DA590D8-EFFF-4932-9308-EACF43A946B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D75C168-7D1A-4B94-B6CC-AEBE7F429AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1216,7 +1216,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{BBEC7189-69EF-41F7-B767-D95EBFD6D62F}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{FEAC00CC-3DBF-453B-8C04-F2A1865E98ED}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1246,10 +1246,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F0486B-3931-44E8-815B-7C9C7C0EF3CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19116163-2A22-435C-8D42-CA7BDCBCA522}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1287,7 +1287,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{189B1247-1CBB-4E4E-8262-849C6EB939D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{193BB0F9-407C-4922-A9BD-B14D757BC3D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,7 +1350,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D767A65-4EBF-4D14-A6E4-C23FC10A8208}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{302EA9A9-016D-4E00-8C54-DB60C2257372}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1369,7 +1369,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B1AAC3C-88AE-1189-0C0F-2FAD5E68E8BD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78657290-A059-FC36-7EDC-848F3AE841B1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1418,7 +1418,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16985C94-91E9-3AB8-BB9E-AAEFF2162591}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92C40D73-3C44-077F-BAF7-AC597D56BCFE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1437,7 +1437,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{082B8558-13B3-F251-8574-7A496E1A7351}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FCEC111-C0F8-9E74-DAB3-BBF96B6613C5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1468,7 +1468,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA955A30-FF14-7163-EEF1-00723BDFBB52}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B341F9B-CFB2-8B9E-89EA-510DF80706B0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1499,7 +1499,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A22C3C1-E3E9-3ABF-A61F-964AFDCC1810}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD01F3D9-484B-4E60-1BA4-915ED3EDA721}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1542,7 +1542,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDA2642B-9A76-4B59-A369-9548DA0BCC09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F92E5F4A-736A-41A2-B8C6-8D71EB14225D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1580,7 +1580,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0137B555-0691-4D09-A4FE-4D39DE633511}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8DCB985-32D9-4DE8-B3E8-1405A0A35D73}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1623,7 +1623,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7C5D837-0CEB-471A-AB6D-286B88C920A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B1E4089-A648-4707-B45D-343C7A427915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1936,7 +1936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757EC95C-D1F4-42BC-A95D-E959F75EA1EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACBB976-A196-4418-B401-B9E399AAF96E}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>